<commit_message>
plumbing sql done for cold water and waste water
</commit_message>
<xml_diff>
--- a/data/plumInfoall.xlsx
+++ b/data/plumInfoall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\material-database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C72F949-A4FB-4726-9BA8-9490232226E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607AA280-37EF-4C98-A6D9-A99858C80238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{A0BBE691-86F4-4964-8F22-F4C94C854054}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{A0BBE691-86F4-4964-8F22-F4C94C854054}"/>
   </bookViews>
   <sheets>
     <sheet name="size" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="brand" sheetId="4" r:id="rId4"/>
     <sheet name="fitting" sheetId="2" r:id="rId5"/>
     <sheet name="fittingInfo" sheetId="6" r:id="rId6"/>
+    <sheet name="plumTypeEnd" sheetId="8" r:id="rId7"/>
+    <sheet name="pipeinfo" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="193">
   <si>
     <t>20mm</t>
   </si>
@@ -375,12 +377,6 @@
     <t xml:space="preserve"> uPVC PNT 7</t>
   </si>
   <si>
-    <t xml:space="preserve"> uPVC CLASS 4.0 SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> uPVCCLASS 2.5 SS</t>
-  </si>
-  <si>
     <t>uPVC Drainage (special) SS</t>
   </si>
   <si>
@@ -616,6 +612,36 @@
   </si>
   <si>
     <t>plumTypeId</t>
+  </si>
+  <si>
+    <t>PlumPipeLengthMetric</t>
+  </si>
+  <si>
+    <t>plumPipeLengthImperial</t>
+  </si>
+  <si>
+    <t>plumPipeEndType</t>
+  </si>
+  <si>
+    <t>PE - Plain Ended</t>
+  </si>
+  <si>
+    <t>SS - Solvent Socketed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> uPVC CLASS 4.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> uPVCCLASS 2.5</t>
+  </si>
+  <si>
+    <t>160mm</t>
+  </si>
+  <si>
+    <t>6"</t>
+  </si>
+  <si>
+    <t>6\"</t>
   </si>
 </sst>
 </file>
@@ -979,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1537CBF8-F71A-411B-9DB0-DEF6645F17DF}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A33"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1052,7 @@
         <v>"20mm"</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>_xlfn.CONCAT(""""&amp;E2&amp;"""")</f>
@@ -1037,8 +1063,8 @@
         <v>("20mm", "1/2\"")</v>
       </c>
       <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES",(TRANSPOSE(G2:G33)&amp;","))</f>
-        <v>INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES("20mm", "1/2\""),("25mm", "3/4\""),("32mm", "1\""),("40mm", "1 1/4\""),("50mm", "1 1/2\""),("63mm", "2\""),("75mm", "2 1/2\""),("90mm", "3\""),("110mm", "4\""),("25mm x 20mm", "3/4\" x 1/2\""),("32mm x 20mm", "1\" x 1/2\""),("32mm x 25mm", "1\" x 3/4\""),("40mm x 20mm", "1 1/4\" x 1/2\""),("40mm x 25mm", "1 1/4\" x 3/4\""),("40mm x 32mm", "1 1/4\" x 1\""),("50mmx 20mm", "1 1/2\" x 1/2\""),("50mm x 25mm", "1 1/2\" x 3/4\""),("50mm x 32mm", "1 1/2\" x 1\""),("50mm x 40mm", "1 1/2\" x 1 1/4\""),("63mm x 20mm", "2\" x 1/2\""),("63mm x 25mm", "2\" x 3/4\""),("63mm x 32mm", "2\" x 1\""),("63mm x 40mm", "2\" x 1 1/4\""),("63mm x 50mm", "2\" x 1 1/2\""),("90mm x 40mm", "3\" x 1 1/4\""),("90mm x 50mm", "3\" x 1 1/2\""),("90mm x 63mm", "3\" x 2\""),("90mm x 75mm", "3\" x 2 1/2\""),("110mm x 50mm", "4\" x 1 1/2\""),("110mm x 63mm", "4\" x 2\""),("110mm x 75mm", "4\" x 2 1/2\""),("110mm x 90mm", "4\" x 3\""),</v>
+        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES",(TRANSPOSE(G2:G34)&amp;","))</f>
+        <v>INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES("20mm", "1/2\""),("25mm", "3/4\""),("32mm", "1\""),("40mm", "1 1/4\""),("50mm", "1 1/2\""),("63mm", "2\""),("75mm", "2 1/2\""),("90mm", "3\""),("110mm", "4\""),("25mm x 20mm", "3/4\" x 1/2\""),("32mm x 20mm", "1\" x 1/2\""),("32mm x 25mm", "1\" x 3/4\""),("40mm x 20mm", "1 1/4\" x 1/2\""),("40mm x 25mm", "1 1/4\" x 3/4\""),("40mm x 32mm", "1 1/4\" x 1\""),("50mmx 20mm", "1 1/2\" x 1/2\""),("50mm x 25mm", "1 1/2\" x 3/4\""),("50mm x 32mm", "1 1/2\" x 1\""),("50mm x 40mm", "1 1/2\" x 1 1/4\""),("63mm x 20mm", "2\" x 1/2\""),("63mm x 25mm", "2\" x 3/4\""),("63mm x 32mm", "2\" x 1\""),("63mm x 40mm", "2\" x 1 1/4\""),("63mm x 50mm", "2\" x 1 1/2\""),("90mm x 40mm", "3\" x 1 1/4\""),("90mm x 50mm", "3\" x 1 1/2\""),("90mm x 63mm", "3\" x 2\""),("90mm x 75mm", "3\" x 2 1/2\""),("110mm x 50mm", "4\" x 1 1/2\""),("110mm x 63mm", "4\" x 2\""),("110mm x 75mm", "4\" x 2 1/2\""),("110mm x 90mm", "4\" x 3\""),("160mm", "6\""),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1056,7 +1082,7 @@
         <v>"25mm"</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" ref="F3:F33" si="2">_xlfn.CONCAT(""""&amp;E3&amp;"""")</f>
@@ -1082,7 +1108,7 @@
         <v>"32mm"</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1108,7 +1134,7 @@
         <v>"40mm"</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1134,7 +1160,7 @@
         <v>"50mm"</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1160,7 +1186,7 @@
         <v>"63mm"</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1186,7 +1212,7 @@
         <v>"75mm"</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1212,7 +1238,7 @@
         <v>"90mm"</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1238,7 +1264,7 @@
         <v>"110mm"</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1264,7 +1290,7 @@
         <v>"25mm x 20mm"</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1290,7 +1316,7 @@
         <v>"32mm x 20mm"</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F12" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1316,7 +1342,7 @@
         <v>"32mm x 25mm"</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F13" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1342,7 +1368,7 @@
         <v>"40mm x 20mm"</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F14" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1368,7 +1394,7 @@
         <v>"40mm x 25mm"</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F15" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1394,7 +1420,7 @@
         <v>"40mm x 32mm"</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1420,7 +1446,7 @@
         <v>"50mmx 20mm"</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1446,7 +1472,7 @@
         <v>"50mm x 25mm"</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1472,7 +1498,7 @@
         <v>"50mm x 32mm"</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F19" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1498,7 +1524,7 @@
         <v>"50mm x 40mm"</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F20" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1524,7 +1550,7 @@
         <v>"63mm x 20mm"</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F21" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1550,7 +1576,7 @@
         <v>"63mm x 25mm"</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F22" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1576,7 +1602,7 @@
         <v>"63mm x 32mm"</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F23" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1602,7 +1628,7 @@
         <v>"63mm x 40mm"</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F24" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1628,7 +1654,7 @@
         <v>"63mm x 50mm"</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F25" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1654,7 +1680,7 @@
         <v>"90mm x 40mm"</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F26" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1680,7 +1706,7 @@
         <v>"90mm x 50mm"</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F27" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1706,7 +1732,7 @@
         <v>"90mm x 63mm"</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F28" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1732,7 +1758,7 @@
         <v>"90mm x 75mm"</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F29" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1758,7 +1784,7 @@
         <v>"110mm x 50mm"</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F30" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1784,7 +1810,7 @@
         <v>"110mm x 63mm"</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F31" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1810,7 +1836,7 @@
         <v>"110mm x 75mm"</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F32" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1836,7 +1862,7 @@
         <v>"110mm x 90mm"</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F33" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1845,6 +1871,32 @@
       <c r="G33" t="str">
         <f t="shared" si="0"/>
         <v>("110mm x 90mm", "4\" x 3\"")</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" ref="D34" si="3">_xlfn.CONCAT(""""&amp;B34&amp;"""")</f>
+        <v>"160mm"</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f t="shared" ref="F34" si="4">_xlfn.CONCAT(""""&amp;E34&amp;"""")</f>
+        <v>"6\""</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" ref="G34" si="5">_xlfn.CONCAT( "(",D34,", ", F34,")")</f>
+        <v>("160mm", "6\"")</v>
       </c>
     </row>
   </sheetData>
@@ -1857,7 +1909,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1931,7 @@
         <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1890,7 +1942,7 @@
         <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>_xlfn.CONCAT(""""&amp;B2&amp;"""")</f>
@@ -1906,7 +1958,7 @@
       </c>
       <c r="G2" t="str" cm="1">
         <f t="array" ref="G2">_xlfn.CONCAT("INSERT INTO plumgrades (plumGrade,plumStandard) VALUES",(TRANSPOSE(F2:F14)&amp;","))</f>
-        <v>INSERT INTO plumgrades (plumGrade,plumStandard) VALUES("uPVC PNT 14", "SLS 147:2013 "),("uPVC PNT 14 - Fitting", "SLS 659:2015"),(" uPVC PNT 11", "SLS 147:2013 "),(" uPVC PNT 11 - Fitting", "SLS 659:2015"),(" uPVC PNT 12.5 - Fitting", "SLS 659:2016"),(" uPVC PNT 7", "SLS 147:2013 "),(" uPVC CLASS 4.0 SS", "SLS 1325"),(" uPVCCLASS 2.5 SS", "SLS 1325"),("uPVC Drainage - fittings", "SLS 1325"),("uPVC Drainage (special) SS", "SLS 1286"),("Tube Well Pipe SS", "Non-Type"),("Irrigation Pipe SS", "Non-Type"),("CPVC", "IS : 15778"),</v>
+        <v>INSERT INTO plumgrades (plumGrade,plumStandard) VALUES("uPVC PNT 14", "SLS 147:2013 "),("uPVC PNT 14 - Fitting", "SLS 659:2015"),(" uPVC PNT 11", "SLS 147:2013 "),(" uPVC PNT 11 - Fitting", "SLS 659:2015"),(" uPVC PNT 12.5 - Fitting", "SLS 659:2016"),(" uPVC PNT 7", "SLS 147:2013 "),(" uPVC CLASS 4.0 ", "SLS 1325"),(" uPVCCLASS 2.5", "SLS 1325"),("uPVC Drainage - fittings", "SLS 1325"),("uPVC Drainage (special) SS", "SLS 1286"),("Tube Well Pipe SS", "Non-Type"),("Irrigation Pipe SS", "Non-Type"),("CPVC", "IS : 15778"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1914,10 +1966,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
       </c>
       <c r="D3" s="1" t="str">
         <f t="shared" ref="D3:D14" si="0">_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
@@ -1940,7 +1992,7 @@
         <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1960,10 +2012,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1983,10 +2035,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" ref="D6" si="3">_xlfn.CONCAT(""""&amp;B6&amp;"""")</f>
@@ -2009,7 +2061,7 @@
         <v>103</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2029,14 +2081,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>" uPVC CLASS 4.0 SS"</v>
+        <v>" uPVC CLASS 4.0 "</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2044,7 +2096,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
-        <v>(" uPVC CLASS 4.0 SS", "SLS 1325")</v>
+        <v>(" uPVC CLASS 4.0 ", "SLS 1325")</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2052,14 +2104,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>105</v>
+        <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>" uPVCCLASS 2.5 SS"</v>
+        <v>" uPVCCLASS 2.5"</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2067,7 +2119,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
-        <v>(" uPVCCLASS 2.5 SS", "SLS 1325")</v>
+        <v>(" uPVCCLASS 2.5", "SLS 1325")</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2075,10 +2127,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2098,10 +2150,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2124,7 +2176,7 @@
         <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2147,7 +2199,7 @@
         <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2167,10 +2219,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2212,7 +2264,7 @@
         <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2220,7 +2272,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1" t="str">
         <f>_xlfn.CONCAT(""""&amp;B2&amp;"""")</f>
@@ -2240,7 +2292,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" ref="C3:C7" si="0">_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
@@ -2256,7 +2308,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2272,7 +2324,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2288,7 +2340,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2304,7 +2356,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2721,7 +2773,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" ref="C20" si="2">_xlfn.CONCAT(""""&amp;B20&amp;"""")</f>
@@ -2737,7 +2789,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" ref="C21" si="4">_xlfn.CONCAT(""""&amp;B21&amp;"""")</f>
@@ -2881,7 +2933,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2897,7 +2949,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2913,7 +2965,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2929,7 +2981,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2945,7 +2997,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2961,7 +3013,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2977,7 +3029,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2993,7 +3045,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3009,7 +3061,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3025,7 +3077,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3041,7 +3093,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3057,7 +3109,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3073,7 +3125,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3089,7 +3141,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3105,7 +3157,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3121,7 +3173,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3137,7 +3189,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3153,7 +3205,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C47" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3169,7 +3221,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C48" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3188,10 +3240,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8B51A4-0C2E-4883-BC0A-528D5C113E23}">
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,19 +3262,19 @@
         <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" t="s">
         <v>176</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>177</v>
       </c>
-      <c r="D1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" t="s">
-        <v>179</v>
-      </c>
       <c r="F1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3249,8 +3301,8 @@
         <v>(1, 1, 2, 1, 2)</v>
       </c>
       <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES",(TRANSPOSE(G2:G138)&amp;","))</f>
-        <v>INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES(1, 1, 2, 1, 2),(1, 1, 4, 2, 2),(1, 1, 4, 3, 2),(1, 1, 4, 4, 2),(1, 1, 4, 5, 2),(1, 1, 4, 6, 2),(1, 1, 4, 7, 2),(1, 1, 4, 8, 2),(1, 1, 4, 9, 2),(2, 1, 2, 1, 2),(2, 1, 4, 2, 2),(2, 1, 4, 3, 2),(2, 1, 4, 4, 2),(2, 1, 4, 5, 2),(2, 1, 4, 6, 2),(2, 1, 4, 7, 2),(2, 1, 4, 8, 2),(2, 1, 4, 9, 2),(3, 1, 2, 1, 2),(3, 1, 4, 2, 2),(3, 1, 4, 3, 2),(3, 1, 4, 4, 2),(3, 1, 4, 5, 2),(3, 1, 4, 6, 2),(3, 1, 4, 7, 2),(3, 1, 4, 8, 2),(3, 1, 4, 9, 2),(4, 1, 2, 1, 2),(4, 1, 4, 2, 2),(4, 1, 4, 3, 2),(4, 1, 4, 4, 2),(4, 1, 4, 5, 2),(4, 1, 4, 6, 2),(4, 1, 4, 7, 2),(4, 1, 4, 8, 2),(4, 1, 4, 9, 2),(5, 1, 2, 1, 2),(5, 1, 4, 2, 2),(5, 1, 4, 3, 2),(5, 1, 4, 4, 2),(5, 1, 4, 5, 2),(5, 1, 4, 6, 2),(5, 1, 4, 7, 2),(5, 1, 4, 8, 2),(5, 1, 4, 9, 2),(6, 1, 2, 1, 2),(6, 1, 4, 2, 2),(6, 1, 4, 3, 2),(6, 1, 4, 4, 2),(6, 1, 4, 5, 2),(6, 1, 4, 6, 2),(6, 1, 4, 7, 2),(6, 1, 4, 8, 2),(6, 1, 4, 9, 2),(7, 1, 2, 1, 2),(7, 1, 4, 2, 2),(7, 1, 4, 3, 2),(7, 1, 4, 4, 2),(7, 1, 4, 5, 2),(7, 1, 4, 6, 2),(7, 1, 4, 7, 2),(7, 1, 4, 8, 2),(7, 1, 4, 9, 2),(8, 1, 2, 1, 2),(8, 1, 4, 2, 2),(8, 1, 4, 3, 2),(8, 1, 4, 4, 2),(8, 1, 4, 5, 2),(8, 1, 4, 6, 2),(8, 1, 4, 7, 2),(8, 1, 4, 8, 2),(8, 1, 4, 9, 2),(9, 1, 2, 1, 2),(9, 1, 4, 2, 2),(9, 1, 4, 3, 2),(9, 1, 4, 4, 2),(9, 1, 4, 5, 2),(9, 1, 4, 6, 2),(10, 1, 4, 10, 2),(10, 1, 4, 11, 2),(10, 1, 4, 12, 2),(10, 1, 4, 13, 2),(10, 1, 4, 14, 2),(10, 1, 4, 15, 2),(10, 1, 4, 16, 2),(10, 1, 4, 17, 2),(10, 1, 4, 18, 2),(10, 1, 4, 19, 2),(10, 1, 4, 20, 2),(10, 1, 4, 21, 2),(10, 1, 4, 22, 2),(10, 1, 4, 23, 2),(10, 1, 4, 24, 2),(10, 1, 4, 25, 2),(10, 1, 4, 26, 2),(10, 1, 4, 27, 2),(10, 1, 4, 28, 2),(10, 1, 4, 29, 2),(10, 1, 4, 30, 2),(10, 1, 4, 31, 2),(10, 1, 4, 32, 2),(11, 1, 4, 10, 2),(11, 1, 4, 11, 2),(11, 1, 4, 12, 2),(11, 1, 4, 13, 2),(11, 1, 4, 14, 2),(11, 1, 4, 15, 2),(11, 1, 4, 16, 2),(11, 1, 4, 17, 2),(11, 1, 4, 18, 2),(11, 1, 4, 19, 2),(11, 1, 4, 20, 2),(11, 1, 4, 21, 2),(11, 1, 4, 22, 2),(11, 1, 4, 23, 2),(11, 1, 4, 24, 2),(11, 1, 4, 25, 2),(11, 1, 4, 26, 2),(11, 1, 4, 27, 2),(11, 1, 4, 28, 2),(11, 1, 4, 29, 2),(11, 1, 4, 30, 2),(11, 1, 4, 31, 2),(11, 1, 4, 32, 2),(12, 1, 4, 10, 2),(13, 1, 4, 11, 2),(14, 1, 2, 1, 2),(15, 1, 2, 1, 2),(16, 1, 2, 1, 2),(17, 1, 2, 1, 2),(18, 1, 2, 1, 2),(19, 1, 5, 10, 2),(19, 1, 5, 11, 2),(20, 1, 5, 10, 2),(21, 1, 2, 1, 2),(21, 1, 4, 2, 2),(21, 1, 4, 3, 2),</v>
+        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES",(TRANSPOSE(G2:G176)&amp;","))</f>
+        <v>INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES(1, 1, 2, 1, 2),(1, 1, 4, 2, 2),(1, 1, 4, 3, 2),(1, 1, 4, 4, 2),(1, 1, 4, 5, 2),(1, 1, 4, 6, 2),(1, 1, 4, 7, 2),(1, 1, 4, 8, 2),(1, 1, 4, 9, 2),(2, 1, 2, 1, 2),(2, 1, 4, 2, 2),(2, 1, 4, 3, 2),(2, 1, 4, 4, 2),(2, 1, 4, 5, 2),(2, 1, 4, 6, 2),(2, 1, 4, 7, 2),(2, 1, 4, 8, 2),(2, 1, 4, 9, 2),(3, 1, 2, 1, 2),(3, 1, 4, 2, 2),(3, 1, 4, 3, 2),(3, 1, 4, 4, 2),(3, 1, 4, 5, 2),(3, 1, 4, 6, 2),(3, 1, 4, 7, 2),(3, 1, 4, 8, 2),(3, 1, 4, 9, 2),(4, 1, 2, 1, 2),(4, 1, 4, 2, 2),(4, 1, 4, 3, 2),(4, 1, 4, 4, 2),(4, 1, 4, 5, 2),(4, 1, 4, 6, 2),(4, 1, 4, 7, 2),(4, 1, 4, 8, 2),(4, 1, 4, 9, 2),(5, 1, 2, 1, 2),(5, 1, 4, 2, 2),(5, 1, 4, 3, 2),(5, 1, 4, 4, 2),(5, 1, 4, 5, 2),(5, 1, 4, 6, 2),(5, 1, 4, 7, 2),(5, 1, 4, 8, 2),(5, 1, 4, 9, 2),(6, 1, 2, 1, 2),(6, 1, 4, 2, 2),(6, 1, 4, 3, 2),(6, 1, 4, 4, 2),(6, 1, 4, 5, 2),(6, 1, 4, 6, 2),(6, 1, 4, 7, 2),(6, 1, 4, 8, 2),(6, 1, 4, 9, 2),(7, 1, 2, 1, 2),(7, 1, 4, 2, 2),(7, 1, 4, 3, 2),(7, 1, 4, 4, 2),(7, 1, 4, 5, 2),(7, 1, 4, 6, 2),(7, 1, 4, 7, 2),(7, 1, 4, 8, 2),(7, 1, 4, 9, 2),(8, 1, 2, 1, 2),(8, 1, 4, 2, 2),(8, 1, 4, 3, 2),(8, 1, 4, 4, 2),(8, 1, 4, 5, 2),(8, 1, 4, 6, 2),(8, 1, 4, 7, 2),(8, 1, 4, 8, 2),(8, 1, 4, 9, 2),(9, 1, 2, 1, 2),(9, 1, 4, 2, 2),(9, 1, 4, 3, 2),(9, 1, 4, 4, 2),(9, 1, 4, 5, 2),(9, 1, 4, 6, 2),(10, 1, 4, 10, 2),(10, 1, 4, 11, 2),(10, 1, 4, 12, 2),(10, 1, 4, 13, 2),(10, 1, 4, 14, 2),(10, 1, 4, 15, 2),(10, 1, 4, 16, 2),(10, 1, 4, 17, 2),(10, 1, 4, 18, 2),(10, 1, 4, 19, 2),(10, 1, 4, 20, 2),(10, 1, 4, 21, 2),(10, 1, 4, 22, 2),(10, 1, 4, 23, 2),(10, 1, 4, 24, 2),(10, 1, 4, 25, 2),(10, 1, 4, 26, 2),(10, 1, 4, 27, 2),(10, 1, 4, 28, 2),(10, 1, 4, 29, 2),(10, 1, 4, 30, 2),(10, 1, 4, 31, 2),(10, 1, 4, 32, 2),(11, 1, 4, 10, 2),(11, 1, 4, 11, 2),(11, 1, 4, 12, 2),(11, 1, 4, 13, 2),(11, 1, 4, 14, 2),(11, 1, 4, 15, 2),(11, 1, 4, 16, 2),(11, 1, 4, 17, 2),(11, 1, 4, 18, 2),(11, 1, 4, 19, 2),(11, 1, 4, 20, 2),(11, 1, 4, 21, 2),(11, 1, 4, 22, 2),(11, 1, 4, 23, 2),(11, 1, 4, 24, 2),(11, 1, 4, 25, 2),(11, 1, 4, 26, 2),(11, 1, 4, 27, 2),(11, 1, 4, 28, 2),(11, 1, 4, 29, 2),(11, 1, 4, 30, 2),(11, 1, 4, 31, 2),(11, 1, 4, 32, 2),(12, 1, 4, 10, 2),(13, 1, 4, 11, 2),(14, 1, 2, 1, 2),(15, 1, 2, 1, 2),(16, 1, 2, 1, 2),(17, 1, 2, 1, 2),(18, 1, 2, 1, 2),(19, 1, 5, 10, 2),(19, 1, 5, 11, 2),(20, 1, 5, 10, 2),(21, 1, 2, 1, 2),(21, 1, 4, 2, 2),(21, 1, 4, 3, 2),(9, 1, 9, 4, 4),(9, 1, 9, 5, 4),(9, 1, 9, 6, 4),(9, 1, 9, 9, 4),(6, 1, 9, 4, 4),(6, 1, 9, 5, 4),(6, 1, 9, 6, 4),(6, 1, 9, 9, 4),(5, 1, 9, 4, 4),(5, 1, 9, 5, 4),(5, 1, 9, 6, 4),(5, 1, 9, 9, 4),(22, 1, 9, 4, 4),(22, 1, 9, 5, 4),(22, 1, 9, 9, 4),(23, 1, 9, 4, 4),(23, 1, 9, 5, 4),(23, 1, 9, 6, 4),(23, 1, 9, 9, 4),(24, 1, 9, 4, 4),(24, 1, 9, 5, 4),(24, 1, 9, 6, 4),(24, 1, 9, 9, 4),(25, 1, 9, 4, 4),(25, 1, 9, 5, 4),(25, 1, 9, 6, 4),(25, 1, 9, 9, 4),(26, 1, 9, 4, 4),(26, 1, 9, 5, 4),(26, 1, 9, 6, 4),(26, 1, 9, 9, 4),(27, 1, 9, 4, 4),(27, 1, 9, 5, 4),(27, 1, 9, 9, 4),(28, 1, 9, 4, 4),(28, 1, 9, 5, 4),(28, 1, 9, 6, 4),(28, 1, 9, 9, 4),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6345,7 +6397,7 @@
         <v>2</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" ref="G131:G138" si="2">_xlfn.CONCAT( "(",B131,", ", C131,", ", D131,", ", E131,", ", F131,")")</f>
+        <f t="shared" ref="G131:G176" si="2">_xlfn.CONCAT( "(",B131,", ", C131,", ", D131,", ", E131,", ", F131,")")</f>
         <v>(17, 1, 2, 1, 2)</v>
       </c>
     </row>
@@ -6515,6 +6567,1998 @@
       <c r="G138" t="str">
         <f t="shared" si="2"/>
         <v>(21, 1, 4, 3, 2)</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>9</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>9</v>
+      </c>
+      <c r="E139">
+        <v>4</v>
+      </c>
+      <c r="F139">
+        <v>4</v>
+      </c>
+      <c r="G139" t="str">
+        <f t="shared" si="2"/>
+        <v>(9, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>9</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>9</v>
+      </c>
+      <c r="E140">
+        <v>5</v>
+      </c>
+      <c r="F140">
+        <v>4</v>
+      </c>
+      <c r="G140" t="str">
+        <f t="shared" si="2"/>
+        <v>(9, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>9</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>9</v>
+      </c>
+      <c r="E141">
+        <v>6</v>
+      </c>
+      <c r="F141">
+        <v>4</v>
+      </c>
+      <c r="G141" t="str">
+        <f t="shared" si="2"/>
+        <v>(9, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>9</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>9</v>
+      </c>
+      <c r="E142">
+        <v>9</v>
+      </c>
+      <c r="F142">
+        <v>4</v>
+      </c>
+      <c r="G142" t="str">
+        <f t="shared" si="2"/>
+        <v>(9, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>9</v>
+      </c>
+      <c r="E143">
+        <v>4</v>
+      </c>
+      <c r="F143">
+        <v>4</v>
+      </c>
+      <c r="G143" t="str">
+        <f t="shared" si="2"/>
+        <v>(6, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>6</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <v>9</v>
+      </c>
+      <c r="E144">
+        <v>5</v>
+      </c>
+      <c r="F144">
+        <v>4</v>
+      </c>
+      <c r="G144" t="str">
+        <f t="shared" si="2"/>
+        <v>(6, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>6</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <v>9</v>
+      </c>
+      <c r="E145">
+        <v>6</v>
+      </c>
+      <c r="F145">
+        <v>4</v>
+      </c>
+      <c r="G145" t="str">
+        <f t="shared" si="2"/>
+        <v>(6, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>6</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>9</v>
+      </c>
+      <c r="E146">
+        <v>9</v>
+      </c>
+      <c r="F146">
+        <v>4</v>
+      </c>
+      <c r="G146" t="str">
+        <f t="shared" si="2"/>
+        <v>(6, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>5</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>9</v>
+      </c>
+      <c r="E147">
+        <v>4</v>
+      </c>
+      <c r="F147">
+        <v>4</v>
+      </c>
+      <c r="G147" t="str">
+        <f t="shared" si="2"/>
+        <v>(5, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>5</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>9</v>
+      </c>
+      <c r="E148">
+        <v>5</v>
+      </c>
+      <c r="F148">
+        <v>4</v>
+      </c>
+      <c r="G148" t="str">
+        <f t="shared" si="2"/>
+        <v>(5, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>5</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>9</v>
+      </c>
+      <c r="E149">
+        <v>6</v>
+      </c>
+      <c r="F149">
+        <v>4</v>
+      </c>
+      <c r="G149" t="str">
+        <f t="shared" si="2"/>
+        <v>(5, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>5</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>9</v>
+      </c>
+      <c r="E150">
+        <v>9</v>
+      </c>
+      <c r="F150">
+        <v>4</v>
+      </c>
+      <c r="G150" t="str">
+        <f t="shared" si="2"/>
+        <v>(5, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>22</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151">
+        <v>9</v>
+      </c>
+      <c r="E151">
+        <v>4</v>
+      </c>
+      <c r="F151">
+        <v>4</v>
+      </c>
+      <c r="G151" t="str">
+        <f t="shared" si="2"/>
+        <v>(22, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152">
+        <v>22</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>9</v>
+      </c>
+      <c r="E152">
+        <v>5</v>
+      </c>
+      <c r="F152">
+        <v>4</v>
+      </c>
+      <c r="G152" t="str">
+        <f t="shared" si="2"/>
+        <v>(22, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153">
+        <v>22</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>9</v>
+      </c>
+      <c r="E153">
+        <v>9</v>
+      </c>
+      <c r="F153">
+        <v>4</v>
+      </c>
+      <c r="G153" t="str">
+        <f t="shared" si="2"/>
+        <v>(22, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154">
+        <v>23</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+      <c r="D154">
+        <v>9</v>
+      </c>
+      <c r="E154">
+        <v>4</v>
+      </c>
+      <c r="F154">
+        <v>4</v>
+      </c>
+      <c r="G154" t="str">
+        <f t="shared" si="2"/>
+        <v>(23, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155">
+        <v>23</v>
+      </c>
+      <c r="C155">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>9</v>
+      </c>
+      <c r="E155">
+        <v>5</v>
+      </c>
+      <c r="F155">
+        <v>4</v>
+      </c>
+      <c r="G155" t="str">
+        <f t="shared" si="2"/>
+        <v>(23, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156">
+        <v>23</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>9</v>
+      </c>
+      <c r="E156">
+        <v>6</v>
+      </c>
+      <c r="F156">
+        <v>4</v>
+      </c>
+      <c r="G156" t="str">
+        <f t="shared" si="2"/>
+        <v>(23, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157">
+        <v>23</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="D157">
+        <v>9</v>
+      </c>
+      <c r="E157">
+        <v>9</v>
+      </c>
+      <c r="F157">
+        <v>4</v>
+      </c>
+      <c r="G157" t="str">
+        <f t="shared" si="2"/>
+        <v>(23, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158">
+        <v>24</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>9</v>
+      </c>
+      <c r="E158">
+        <v>4</v>
+      </c>
+      <c r="F158">
+        <v>4</v>
+      </c>
+      <c r="G158" t="str">
+        <f t="shared" si="2"/>
+        <v>(24, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159">
+        <v>24</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>9</v>
+      </c>
+      <c r="E159">
+        <v>5</v>
+      </c>
+      <c r="F159">
+        <v>4</v>
+      </c>
+      <c r="G159" t="str">
+        <f t="shared" si="2"/>
+        <v>(24, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160">
+        <v>24</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>9</v>
+      </c>
+      <c r="E160">
+        <v>6</v>
+      </c>
+      <c r="F160">
+        <v>4</v>
+      </c>
+      <c r="G160" t="str">
+        <f t="shared" si="2"/>
+        <v>(24, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>24</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>9</v>
+      </c>
+      <c r="E161">
+        <v>9</v>
+      </c>
+      <c r="F161">
+        <v>4</v>
+      </c>
+      <c r="G161" t="str">
+        <f t="shared" si="2"/>
+        <v>(24, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>25</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>9</v>
+      </c>
+      <c r="E162">
+        <v>4</v>
+      </c>
+      <c r="F162">
+        <v>4</v>
+      </c>
+      <c r="G162" t="str">
+        <f t="shared" si="2"/>
+        <v>(25, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163">
+        <v>25</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>9</v>
+      </c>
+      <c r="E163">
+        <v>5</v>
+      </c>
+      <c r="F163">
+        <v>4</v>
+      </c>
+      <c r="G163" t="str">
+        <f t="shared" si="2"/>
+        <v>(25, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164">
+        <v>25</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <v>9</v>
+      </c>
+      <c r="E164">
+        <v>6</v>
+      </c>
+      <c r="F164">
+        <v>4</v>
+      </c>
+      <c r="G164" t="str">
+        <f t="shared" si="2"/>
+        <v>(25, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165">
+        <v>25</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+      <c r="D165">
+        <v>9</v>
+      </c>
+      <c r="E165">
+        <v>9</v>
+      </c>
+      <c r="F165">
+        <v>4</v>
+      </c>
+      <c r="G165" t="str">
+        <f t="shared" si="2"/>
+        <v>(25, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166">
+        <v>26</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>9</v>
+      </c>
+      <c r="E166">
+        <v>4</v>
+      </c>
+      <c r="F166">
+        <v>4</v>
+      </c>
+      <c r="G166" t="str">
+        <f t="shared" si="2"/>
+        <v>(26, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167">
+        <v>26</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>9</v>
+      </c>
+      <c r="E167">
+        <v>5</v>
+      </c>
+      <c r="F167">
+        <v>4</v>
+      </c>
+      <c r="G167" t="str">
+        <f t="shared" si="2"/>
+        <v>(26, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>26</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168">
+        <v>9</v>
+      </c>
+      <c r="E168">
+        <v>6</v>
+      </c>
+      <c r="F168">
+        <v>4</v>
+      </c>
+      <c r="G168" t="str">
+        <f t="shared" si="2"/>
+        <v>(26, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169">
+        <v>26</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>9</v>
+      </c>
+      <c r="E169">
+        <v>9</v>
+      </c>
+      <c r="F169">
+        <v>4</v>
+      </c>
+      <c r="G169" t="str">
+        <f t="shared" si="2"/>
+        <v>(26, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>27</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>9</v>
+      </c>
+      <c r="E170">
+        <v>4</v>
+      </c>
+      <c r="F170">
+        <v>4</v>
+      </c>
+      <c r="G170" t="str">
+        <f t="shared" si="2"/>
+        <v>(27, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>27</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>9</v>
+      </c>
+      <c r="E171">
+        <v>5</v>
+      </c>
+      <c r="F171">
+        <v>4</v>
+      </c>
+      <c r="G171" t="str">
+        <f t="shared" si="2"/>
+        <v>(27, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>27</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>9</v>
+      </c>
+      <c r="E172">
+        <v>9</v>
+      </c>
+      <c r="F172">
+        <v>4</v>
+      </c>
+      <c r="G172" t="str">
+        <f t="shared" si="2"/>
+        <v>(27, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173">
+        <v>28</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>9</v>
+      </c>
+      <c r="E173">
+        <v>4</v>
+      </c>
+      <c r="F173">
+        <v>4</v>
+      </c>
+      <c r="G173" t="str">
+        <f t="shared" si="2"/>
+        <v>(28, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174">
+        <v>28</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="D174">
+        <v>9</v>
+      </c>
+      <c r="E174">
+        <v>5</v>
+      </c>
+      <c r="F174">
+        <v>4</v>
+      </c>
+      <c r="G174" t="str">
+        <f t="shared" si="2"/>
+        <v>(28, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175">
+        <v>28</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
+      <c r="D175">
+        <v>9</v>
+      </c>
+      <c r="E175">
+        <v>6</v>
+      </c>
+      <c r="F175">
+        <v>4</v>
+      </c>
+      <c r="G175" t="str">
+        <f t="shared" si="2"/>
+        <v>(28, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>28</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>9</v>
+      </c>
+      <c r="E176">
+        <v>9</v>
+      </c>
+      <c r="F176">
+        <v>4</v>
+      </c>
+      <c r="G176" t="str">
+        <f t="shared" si="2"/>
+        <v>(28, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6067A96B-A56E-4CC3-9E7D-BF79F93DE18D}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>_xlfn.CONCAT(""""&amp;B2&amp;"""")</f>
+        <v>"PE - Plain Ended"</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>_xlfn.CONCAT( "(",C2,")")</f>
+        <v>("PE - Plain Ended")</v>
+      </c>
+      <c r="E2" t="str" cm="1">
+        <f t="array" ref="E2">_xlfn.CONCAT("INSERT INTO plumpipeendtypes (plumPipeEndType) VALUES",(TRANSPOSE(D2:D3)&amp;","))</f>
+        <v>INSERT INTO plumpipeendtypes (plumPipeEndType) VALUES("PE - Plain Ended"),("SS - Solvent Socketed"),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
+        <v>"SS - Solvent Socketed"</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>_xlfn.CONCAT( "(",C3,")")</f>
+        <v>("SS - Solvent Socketed")</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD72405-4BAA-4BE0-9E9A-35EF3BE8961C}">
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>G2*3.28</f>
+        <v>13.12</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xlfn.CONCAT( "(",B2,", ", C2,", ", D2,", ", E2,", ", F2,", ", G2,", ", H2,")")</f>
+        <v>(1, 1, 1, 1, 1, 4, 13.12)</v>
+      </c>
+      <c r="J2" t="str" cm="1">
+        <f t="array" ref="J2">_xlfn.CONCAT("INSERT INTO plumpipeinfos (plumGradeId,plumSizeId,plumBrandId,plumTypeId,plumPipeEndType,PlumPipeLengthMetric,plumPipeLengthImperial) VALUES",(TRANSPOSE(I2:I32)&amp;","))</f>
+        <v>INSERT INTO plumpipeinfos (plumGradeId,plumSizeId,plumBrandId,plumTypeId,plumPipeEndType,PlumPipeLengthMetric,plumPipeLengthImperial) VALUES(1, 1, 1, 1, 1, 4, 13.12),(3, 2, 1, 1, 1, 4, 13.12),(3, 3, 1, 1, 1, 4, 13.12),(3, 4, 1, 1, 1, 4, 13.12),(3, 5, 1, 1, 1, 4, 13.12),(3, 6, 1, 1, 1, 4, 13.12),(3, 7, 1, 1, 1, 4, 13.12),(3, 8, 1, 1, 1, 4, 13.12),(3, 9, 1, 1, 1, 6, 19.68),(6, 2, 1, 1, 1, 4, 13.12),(6, 3, 1, 1, 1, 4, 13.12),(6, 4, 1, 1, 1, 4, 13.12),(6, 5, 1, 1, 1, 4, 13.12),(6, 6, 1, 1, 1, 4, 13.12),(6, 7, 1, 1, 1, 4, 13.12),(6, 8, 1, 1, 1, 4, 13.12),(6, 9, 1, 1, 1, 6, 19.68),(7, 5, 1, 3, 1, 4, 13.12),(7, 6, 1, 3, 1, 4, 13.12),(7, 7, 1, 3, 1, 4, 13.12),(7, 8, 1, 3, 1, 4, 13.12),(7, 9, 1, 3, 1, 6, 19.68),(7, 33, 1, 3, 1, 6, 19.68),(8, 9, 1, 3, 2, 6, 19.68),(8, 33, 1, 3, 2, 6, 19.68),(7, 5, 1, 3, 2, 4, 13.12),(7, 6, 1, 3, 2, 4, 13.12),(7, 7, 1, 3, 2, 4, 13.12),(7, 8, 1, 3, 2, 4, 13.12),(7, 9, 1, 3, 2, 6, 19.68),(7, 33, 1, 3, 2, 6, 19.68),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H32" si="0">G3*3.28</f>
+        <v>13.12</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I32" si="1">_xlfn.CONCAT( "(",B3,", ", C3,", ", D3,", ", E3,", ", F3,", ", G3,", ", H3,")")</f>
+        <v>(3, 2, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 3, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 4, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 5, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 6, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 7, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 8, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 9, 1, 1, 1, 6, 19.68)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 2, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 3, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 4, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 5, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 6, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 7, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 8, 1, 1, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>(6, 9, 1, 1, 1, 6, 19.68)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 5, 1, 3, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 6, 1, 3, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 7, 1, 3, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 8, 1, 3, 1, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 9, 1, 3, 1, 6, 19.68)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 33, 1, 3, 1, 6, 19.68)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v>(8, 9, 1, 3, 2, 6, 19.68)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v>(8, 33, 1, 3, 2, 6, 19.68)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 5, 1, 3, 2, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 6, 1, 3, 2, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 7, 1, 3, 2, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>13.12</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 8, 1, 3, 2, 4, 13.12)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 9, 1, 3, 2, 6, 19.68)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>33</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>6</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>19.68</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="1"/>
+        <v>(7, 33, 1, 3, 2, 6, 19.68)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>